<commit_message>
:alembic: Primeiras analise dos dados
Primeiras analise dos dados
</commit_message>
<xml_diff>
--- a/BD Completo.xlsx
+++ b/BD Completo.xlsx
@@ -3,14 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FE312055-65ED-0349-AA52-6AE4FD76C1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9797D916-2B32-4A31-967A-FF1B0DB1A165}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{FE312055-65ED-0349-AA52-6AE4FD76C1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A492B222-D9E0-4E4D-BED9-D23286104B2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$BR$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2842,6 +2856,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3167,56 +3185,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR378"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="AV9" sqref="AV9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="6" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3428,7 +3447,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -3541,7 +3560,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -3714,7 +3733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -3815,7 +3834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3925,7 +3944,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -4020,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -4199,7 +4218,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -4279,7 +4298,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -4365,7 +4384,7 @@
         <v>-34</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -4535,7 +4554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -4636,7 +4655,7 @@
         <v>-415</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -4716,7 +4735,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -4898,7 +4917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -4999,7 +5018,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -5175,7 +5194,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -5216,7 +5235,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -5399,7 +5418,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -5566,7 +5585,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -5634,7 +5653,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -5732,7 +5751,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -5902,7 +5921,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -5994,7 +6013,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -6077,7 +6096,7 @@
         <v>17.82</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -6178,7 +6197,7 @@
         <v>-33</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -6279,7 +6298,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -6389,7 +6408,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -6475,7 +6494,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -6555,7 +6574,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -6629,7 +6648,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -6715,7 +6734,7 @@
         <v>11.71</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -6798,7 +6817,7 @@
         <v>20.59</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -6878,7 +6897,7 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -6961,7 +6980,7 @@
         <v>13.05</v>
       </c>
     </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -7017,7 +7036,7 @@
         <v>7.61</v>
       </c>
     </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -7103,7 +7122,7 @@
         <v>10.93</v>
       </c>
     </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -7180,7 +7199,7 @@
         <v>7.01</v>
       </c>
     </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -7257,7 +7276,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -7340,7 +7359,7 @@
         <v>16.34</v>
       </c>
     </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -7417,7 +7436,7 @@
         <v>14.57</v>
       </c>
     </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -7488,7 +7507,7 @@
         <v>7.21</v>
       </c>
     </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -7538,7 +7557,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -7618,7 +7637,7 @@
         <v>7.42</v>
       </c>
     </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -7704,7 +7723,7 @@
         <v>7.53</v>
       </c>
     </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -7781,7 +7800,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -7879,7 +7898,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -7983,7 +8002,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -8156,7 +8175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -8248,7 +8267,7 @@
         <v>-342</v>
       </c>
     </row>
-    <row r="49" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>75</v>
       </c>
@@ -8409,7 +8428,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -8570,7 +8589,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="51" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -8722,7 +8741,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="52" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -8865,7 +8884,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -9011,7 +9030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -9124,7 +9143,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>99</v>
       </c>
@@ -9306,7 +9325,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -9407,7 +9426,7 @@
         <v>-813</v>
       </c>
     </row>
-    <row r="57" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>99</v>
       </c>
@@ -9493,7 +9512,7 @@
         <v>9.01</v>
       </c>
     </row>
-    <row r="58" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -9669,7 +9688,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -9773,7 +9792,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="60" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -9844,7 +9863,7 @@
         <v>-179</v>
       </c>
     </row>
-    <row r="61" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -9888,7 +9907,7 @@
         <v>5.1100000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -9965,7 +9984,7 @@
         <v>8.68</v>
       </c>
     </row>
-    <row r="63" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -10057,7 +10076,7 @@
         <v>-187</v>
       </c>
     </row>
-    <row r="64" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -10185,7 +10204,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="65" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -10223,7 +10242,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="66" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -10294,7 +10313,7 @@
         <v>-54</v>
       </c>
     </row>
-    <row r="67" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -10371,7 +10390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -10391,7 +10410,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -10438,7 +10457,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="70" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -10539,7 +10558,7 @@
         <v>-84</v>
       </c>
     </row>
-    <row r="71" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -10718,7 +10737,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -10813,7 +10832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>68</v>
       </c>
@@ -10857,7 +10876,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="74" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -10949,7 +10968,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="75" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -11119,7 +11138,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>68</v>
       </c>
@@ -11295,7 +11314,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>68</v>
       </c>
@@ -11396,7 +11415,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="78" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>68</v>
       </c>
@@ -11464,7 +11483,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>68</v>
       </c>
@@ -11640,7 +11659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>99</v>
       </c>
@@ -11807,7 +11826,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -11881,7 +11900,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>68</v>
       </c>
@@ -11982,7 +12001,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="83" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>99</v>
       </c>
@@ -12077,7 +12096,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="84" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>75</v>
       </c>
@@ -12184,7 +12203,7 @@
         <v>-318</v>
       </c>
     </row>
-    <row r="85" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -12261,7 +12280,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -12371,7 +12390,7 @@
         <v>-870</v>
       </c>
     </row>
-    <row r="87" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -12472,7 +12491,7 @@
         <v>-87</v>
       </c>
     </row>
-    <row r="88" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>75</v>
       </c>
@@ -12654,7 +12673,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>99</v>
       </c>
@@ -12755,7 +12774,7 @@
         <v>-113</v>
       </c>
     </row>
-    <row r="90" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>75</v>
       </c>
@@ -12934,7 +12953,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>75</v>
       </c>
@@ -13035,7 +13054,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="92" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>75</v>
       </c>
@@ -13145,7 +13164,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -13243,7 +13262,7 @@
         <v>-476</v>
       </c>
     </row>
-    <row r="94" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -13347,7 +13366,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="95" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>75</v>
       </c>
@@ -13523,7 +13542,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>68</v>
       </c>
@@ -13627,7 +13646,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="97" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>75</v>
       </c>
@@ -13806,7 +13825,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>99</v>
       </c>
@@ -13907,7 +13926,7 @@
         <v>-52</v>
       </c>
     </row>
-    <row r="99" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -14086,7 +14105,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>68</v>
       </c>
@@ -14163,7 +14182,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>68</v>
       </c>
@@ -14240,7 +14259,7 @@
         <v>-203</v>
       </c>
     </row>
-    <row r="102" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>75</v>
       </c>
@@ -14350,7 +14369,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>75</v>
       </c>
@@ -14529,7 +14548,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>75</v>
       </c>
@@ -14639,7 +14658,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="105" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>75</v>
       </c>
@@ -14809,7 +14828,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="106" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>75</v>
       </c>
@@ -14988,7 +15007,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>75</v>
       </c>
@@ -15167,7 +15186,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="108" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>75</v>
       </c>
@@ -15268,7 +15287,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="109" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>68</v>
       </c>
@@ -15441,7 +15460,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>68</v>
       </c>
@@ -15542,7 +15561,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="111" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>68</v>
       </c>
@@ -15640,7 +15659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>75</v>
       </c>
@@ -15819,7 +15838,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>68</v>
       </c>
@@ -15854,7 +15873,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>68</v>
       </c>
@@ -15925,7 +15944,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="115" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>68</v>
       </c>
@@ -15978,7 +15997,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>68</v>
       </c>
@@ -16052,7 +16071,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>68</v>
       </c>
@@ -16150,7 +16169,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="118" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>99</v>
       </c>
@@ -16263,7 +16282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>68</v>
       </c>
@@ -16367,7 +16386,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="120" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>68</v>
       </c>
@@ -16453,7 +16472,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>68</v>
       </c>
@@ -16551,7 +16570,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>99</v>
       </c>
@@ -16655,7 +16674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>75</v>
       </c>
@@ -16729,7 +16748,7 @@
         <v>-87</v>
       </c>
     </row>
-    <row r="124" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>75</v>
       </c>
@@ -16908,7 +16927,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="125" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>68</v>
       </c>
@@ -16973,7 +16992,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="126" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>75</v>
       </c>
@@ -17152,7 +17171,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="127" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>75</v>
       </c>
@@ -17256,7 +17275,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="128" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>68</v>
       </c>
@@ -17360,7 +17379,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="129" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>99</v>
       </c>
@@ -17470,7 +17489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>75</v>
       </c>
@@ -17646,7 +17665,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>99</v>
       </c>
@@ -17825,7 +17844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>75</v>
       </c>
@@ -18004,7 +18023,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="133" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>75</v>
       </c>
@@ -18108,7 +18127,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="134" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>99</v>
       </c>
@@ -18212,7 +18231,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="135" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>99</v>
       </c>
@@ -18322,7 +18341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>68</v>
       </c>
@@ -18393,7 +18412,7 @@
         <v>-94</v>
       </c>
     </row>
-    <row r="137" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>75</v>
       </c>
@@ -18575,7 +18594,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="138" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>75</v>
       </c>
@@ -18676,7 +18695,7 @@
         <v>-2002</v>
       </c>
     </row>
-    <row r="139" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>68</v>
       </c>
@@ -18741,7 +18760,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="140" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>68</v>
       </c>
@@ -18815,7 +18834,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>75</v>
       </c>
@@ -18928,7 +18947,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="142" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>75</v>
       </c>
@@ -19041,7 +19060,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="143" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>99</v>
       </c>
@@ -19214,7 +19233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>68</v>
       </c>
@@ -19288,7 +19307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>68</v>
       </c>
@@ -19389,7 +19408,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="146" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>68</v>
       </c>
@@ -19475,7 +19494,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="147" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>75</v>
       </c>
@@ -19552,7 +19571,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="148" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>68</v>
       </c>
@@ -19665,7 +19684,7 @@
         <v>-97</v>
       </c>
     </row>
-    <row r="149" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>99</v>
       </c>
@@ -19829,7 +19848,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="150" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>99</v>
       </c>
@@ -19930,7 +19949,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="151" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>75</v>
       </c>
@@ -20106,7 +20125,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="152" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>99</v>
       </c>
@@ -20285,7 +20304,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="153" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>68</v>
       </c>
@@ -20392,7 +20411,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>68</v>
       </c>
@@ -20493,7 +20512,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="155" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>75</v>
       </c>
@@ -20603,7 +20622,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="156" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>75</v>
       </c>
@@ -20695,7 +20714,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="157" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>68</v>
       </c>
@@ -20733,7 +20752,7 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="158" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>99</v>
       </c>
@@ -20912,7 +20931,7 @@
         <v>3664</v>
       </c>
     </row>
-    <row r="159" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>68</v>
       </c>
@@ -21025,7 +21044,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="160" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>68</v>
       </c>
@@ -21195,7 +21214,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="161" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>99</v>
       </c>
@@ -21299,7 +21318,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="162" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>99</v>
       </c>
@@ -21409,7 +21428,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="163" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>75</v>
       </c>
@@ -21588,7 +21607,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="164" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>99</v>
       </c>
@@ -21767,7 +21786,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="165" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>99</v>
       </c>
@@ -21940,7 +21959,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>68</v>
       </c>
@@ -22044,7 +22063,7 @@
         <v>-85</v>
       </c>
     </row>
-    <row r="167" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>99</v>
       </c>
@@ -22223,7 +22242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>75</v>
       </c>
@@ -22324,7 +22343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>75</v>
       </c>
@@ -22506,7 +22525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>99</v>
       </c>
@@ -22670,7 +22689,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="171" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>75</v>
       </c>
@@ -22849,7 +22868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="172" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>68</v>
       </c>
@@ -22932,7 +22951,7 @@
         <v>6.32</v>
       </c>
     </row>
-    <row r="173" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>68</v>
       </c>
@@ -22979,7 +22998,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="174" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>68</v>
       </c>
@@ -23083,7 +23102,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>68</v>
       </c>
@@ -23184,7 +23203,7 @@
         <v>-768</v>
       </c>
     </row>
-    <row r="176" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>68</v>
       </c>
@@ -23243,7 +23262,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="177" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>68</v>
       </c>
@@ -23344,7 +23363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>68</v>
       </c>
@@ -23523,7 +23542,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="179" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>75</v>
       </c>
@@ -23705,7 +23724,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="180" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>68</v>
       </c>
@@ -23869,7 +23888,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="181" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>68</v>
       </c>
@@ -24048,7 +24067,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="182" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>75</v>
       </c>
@@ -24215,7 +24234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>68</v>
       </c>
@@ -24382,7 +24401,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="184" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>68</v>
       </c>
@@ -24486,7 +24505,7 @@
         <v>-43</v>
       </c>
     </row>
-    <row r="185" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>75</v>
       </c>
@@ -24659,7 +24678,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="186" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>99</v>
       </c>
@@ -24826,7 +24845,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="187" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>68</v>
       </c>
@@ -24903,7 +24922,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="188" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>99</v>
       </c>
@@ -25004,7 +25023,7 @@
         <v>-56</v>
       </c>
     </row>
-    <row r="189" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>75</v>
       </c>
@@ -25162,7 +25181,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="190" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>99</v>
       </c>
@@ -25338,7 +25357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>68</v>
       </c>
@@ -25358,7 +25377,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="192" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>75</v>
       </c>
@@ -25543,7 +25562,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="193" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>99</v>
       </c>
@@ -25719,7 +25738,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="194" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>68</v>
       </c>
@@ -25811,7 +25830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>99</v>
       </c>
@@ -25987,7 +26006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="196" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>68</v>
       </c>
@@ -26073,7 +26092,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="197" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>68</v>
       </c>
@@ -26120,7 +26139,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="198" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>68</v>
       </c>
@@ -26212,7 +26231,7 @@
         <v>-132</v>
       </c>
     </row>
-    <row r="199" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>75</v>
       </c>
@@ -26391,7 +26410,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="200" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>68</v>
       </c>
@@ -26489,7 +26508,7 @@
         <v>-167</v>
       </c>
     </row>
-    <row r="201" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>68</v>
       </c>
@@ -26581,7 +26600,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="202" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>99</v>
       </c>
@@ -26730,7 +26749,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="203" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>68</v>
       </c>
@@ -26822,7 +26841,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="204" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>68</v>
       </c>
@@ -26923,7 +26942,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="205" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>68</v>
       </c>
@@ -27018,7 +27037,7 @@
         <v>-1970</v>
       </c>
     </row>
-    <row r="206" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>68</v>
       </c>
@@ -27092,7 +27111,7 @@
         <v>-2051</v>
       </c>
     </row>
-    <row r="207" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>68</v>
       </c>
@@ -27184,7 +27203,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="208" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>99</v>
       </c>
@@ -27363,7 +27382,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="209" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>68</v>
       </c>
@@ -27383,7 +27402,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="210" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>75</v>
       </c>
@@ -27469,7 +27488,7 @@
         <v>10.61</v>
       </c>
     </row>
-    <row r="211" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>75</v>
       </c>
@@ -27648,7 +27667,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="212" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>68</v>
       </c>
@@ -27752,7 +27771,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="213" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>99</v>
       </c>
@@ -27850,7 +27869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="214" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>99</v>
       </c>
@@ -27954,7 +27973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="215" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>68</v>
       </c>
@@ -28133,7 +28152,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="216" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>99</v>
       </c>
@@ -28237,7 +28256,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="217" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>68</v>
       </c>
@@ -28338,7 +28357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>99</v>
       </c>
@@ -28499,7 +28518,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="219" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>68</v>
       </c>
@@ -28603,7 +28622,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="220" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>99</v>
       </c>
@@ -28716,7 +28735,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="221" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>99</v>
       </c>
@@ -28817,7 +28836,7 @@
         <v>-477</v>
       </c>
     </row>
-    <row r="222" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>68</v>
       </c>
@@ -28861,7 +28880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="223" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>68</v>
       </c>
@@ -28959,7 +28978,7 @@
         <v>-297</v>
       </c>
     </row>
-    <row r="224" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>99</v>
       </c>
@@ -29129,7 +29148,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="225" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>75</v>
       </c>
@@ -29305,7 +29324,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="226" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>75</v>
       </c>
@@ -29487,7 +29506,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="227" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>75</v>
       </c>
@@ -29666,7 +29685,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="228" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>68</v>
       </c>
@@ -29848,7 +29867,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="229" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>68</v>
       </c>
@@ -29952,7 +29971,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="230" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>75</v>
       </c>
@@ -30137,7 +30156,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="231" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>68</v>
       </c>
@@ -30214,7 +30233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>75</v>
       </c>
@@ -30399,7 +30418,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="233" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>68</v>
       </c>
@@ -30545,7 +30564,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="234" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>68</v>
       </c>
@@ -30649,7 +30668,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="235" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>68</v>
       </c>
@@ -30726,7 +30745,7 @@
         <v>-11004</v>
       </c>
     </row>
-    <row r="236" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>75</v>
       </c>
@@ -30908,7 +30927,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="237" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>75</v>
       </c>
@@ -31090,7 +31109,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="238" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>75</v>
       </c>
@@ -31266,7 +31285,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="239" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>99</v>
       </c>
@@ -31370,7 +31389,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="240" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>99</v>
       </c>
@@ -31552,7 +31571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>68</v>
       </c>
@@ -31650,7 +31669,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="242" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>99</v>
       </c>
@@ -31742,7 +31761,7 @@
         <v>-381</v>
       </c>
     </row>
-    <row r="243" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>68</v>
       </c>
@@ -31804,7 +31823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>99</v>
       </c>
@@ -31983,7 +32002,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="245" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>68</v>
       </c>
@@ -32087,7 +32106,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="246" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>99</v>
       </c>
@@ -32191,7 +32210,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="247" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>68</v>
       </c>
@@ -32292,7 +32311,7 @@
         <v>-857</v>
       </c>
     </row>
-    <row r="248" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>68</v>
       </c>
@@ -32372,7 +32391,7 @@
         <v>6.42</v>
       </c>
     </row>
-    <row r="249" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>68</v>
       </c>
@@ -32476,7 +32495,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="250" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>99</v>
       </c>
@@ -32577,7 +32596,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="251" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>68</v>
       </c>
@@ -32660,7 +32679,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="252" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>75</v>
       </c>
@@ -32830,7 +32849,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="253" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>99</v>
       </c>
@@ -32928,7 +32947,7 @@
         <v>-123</v>
       </c>
     </row>
-    <row r="254" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>68</v>
       </c>
@@ -33041,7 +33060,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="255" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>99</v>
       </c>
@@ -33208,7 +33227,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="256" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>68</v>
       </c>
@@ -33288,7 +33307,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="257" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>68</v>
       </c>
@@ -33392,7 +33411,7 @@
         <v>2848</v>
       </c>
     </row>
-    <row r="258" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>68</v>
       </c>
@@ -33487,7 +33506,7 @@
         <v>-317</v>
       </c>
     </row>
-    <row r="259" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>68</v>
       </c>
@@ -33654,7 +33673,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="260" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>75</v>
       </c>
@@ -33755,7 +33774,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="261" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>68</v>
       </c>
@@ -33856,7 +33875,7 @@
         <v>-256</v>
       </c>
     </row>
-    <row r="262" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>75</v>
       </c>
@@ -34038,7 +34057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>75</v>
       </c>
@@ -34223,7 +34242,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="264" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>99</v>
       </c>
@@ -34381,7 +34400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>68</v>
       </c>
@@ -34485,7 +34504,7 @@
         <v>-164</v>
       </c>
     </row>
-    <row r="266" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>68</v>
       </c>
@@ -34556,7 +34575,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="267" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>68</v>
       </c>
@@ -34660,7 +34679,7 @@
         <v>-932</v>
       </c>
     </row>
-    <row r="268" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>99</v>
       </c>
@@ -34773,7 +34792,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="269" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>99</v>
       </c>
@@ -34955,7 +34974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="270" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>68</v>
       </c>
@@ -35029,7 +35048,7 @@
         <v>-893</v>
       </c>
     </row>
-    <row r="271" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>68</v>
       </c>
@@ -35094,7 +35113,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="272" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>68</v>
       </c>
@@ -35180,7 +35199,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="273" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>68</v>
       </c>
@@ -35278,7 +35297,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="274" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>68</v>
       </c>
@@ -35349,7 +35368,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>75</v>
       </c>
@@ -35507,7 +35526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>68</v>
       </c>
@@ -35557,7 +35576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>68</v>
       </c>
@@ -35652,7 +35671,7 @@
         <v>-3248</v>
       </c>
     </row>
-    <row r="278" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>68</v>
       </c>
@@ -35822,7 +35841,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="279" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>99</v>
       </c>
@@ -35992,7 +36011,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="280" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>75</v>
       </c>
@@ -36153,7 +36172,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="281" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>75</v>
       </c>
@@ -36305,7 +36324,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="282" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>99</v>
       </c>
@@ -36409,7 +36428,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>99</v>
       </c>
@@ -36495,7 +36514,7 @@
         <v>4.49</v>
       </c>
     </row>
-    <row r="284" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>99</v>
       </c>
@@ -36599,7 +36618,7 @@
         <v>-344</v>
       </c>
     </row>
-    <row r="285" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>99</v>
       </c>
@@ -36772,7 +36791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="286" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>75</v>
       </c>
@@ -36945,7 +36964,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="287" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>68</v>
       </c>
@@ -37058,7 +37077,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="288" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>68</v>
       </c>
@@ -37162,7 +37181,7 @@
         <v>-423</v>
       </c>
     </row>
-    <row r="289" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>68</v>
       </c>
@@ -37212,7 +37231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>75</v>
       </c>
@@ -37367,7 +37386,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="291" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>68</v>
       </c>
@@ -37540,7 +37559,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="292" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>68</v>
       </c>
@@ -37593,7 +37612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="293" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>68</v>
       </c>
@@ -37700,7 +37719,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="294" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>75</v>
       </c>
@@ -37804,7 +37823,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="295" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>99</v>
       </c>
@@ -37902,7 +37921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>68</v>
       </c>
@@ -37973,7 +37992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="297" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>68</v>
       </c>
@@ -38143,7 +38162,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="298" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>75</v>
       </c>
@@ -38325,7 +38344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="299" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>68</v>
       </c>
@@ -38399,7 +38418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="300" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>75</v>
       </c>
@@ -38584,7 +38603,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="301" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>99</v>
       </c>
@@ -38757,7 +38776,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="302" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>68</v>
       </c>
@@ -38849,7 +38868,7 @@
         <v>-65</v>
       </c>
     </row>
-    <row r="303" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>68</v>
       </c>
@@ -38953,7 +38972,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="304" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>68</v>
       </c>
@@ -39048,7 +39067,7 @@
         <v>-754</v>
       </c>
     </row>
-    <row r="305" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>68</v>
       </c>
@@ -39212,7 +39231,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="306" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>68</v>
       </c>
@@ -39385,7 +39404,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="307" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>68</v>
       </c>
@@ -39435,7 +39454,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="308" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>68</v>
       </c>
@@ -39488,7 +39507,7 @@
         <v>541.22</v>
       </c>
     </row>
-    <row r="309" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>68</v>
       </c>
@@ -39592,7 +39611,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="310" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>99</v>
       </c>
@@ -39762,7 +39781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="311" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>75</v>
       </c>
@@ -39935,7 +39954,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="312" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>99</v>
       </c>
@@ -40108,7 +40127,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="313" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>68</v>
       </c>
@@ -40146,7 +40165,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="314" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>68</v>
       </c>
@@ -40196,7 +40215,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="315" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>68</v>
       </c>
@@ -40279,7 +40298,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="316" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>99</v>
       </c>
@@ -40452,7 +40471,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="317" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>99</v>
       </c>
@@ -40625,7 +40644,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="318" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>99</v>
       </c>
@@ -40807,7 +40826,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="319" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>99</v>
       </c>
@@ -40908,7 +40927,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="320" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>99</v>
       </c>
@@ -41078,7 +41097,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="321" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>68</v>
       </c>
@@ -41149,7 +41168,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="322" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>68</v>
       </c>
@@ -41262,7 +41281,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="323" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>68</v>
       </c>
@@ -41327,7 +41346,7 @@
         <v>38243</v>
       </c>
     </row>
-    <row r="324" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>68</v>
       </c>
@@ -41431,7 +41450,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="325" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>99</v>
       </c>
@@ -41604,7 +41623,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="326" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>99</v>
       </c>
@@ -41777,7 +41796,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="327" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>68</v>
       </c>
@@ -41878,7 +41897,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="328" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>68</v>
       </c>
@@ -41982,7 +42001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="329" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>68</v>
       </c>
@@ -42158,7 +42177,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="330" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>99</v>
       </c>
@@ -42328,7 +42347,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="331" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>68</v>
       </c>
@@ -42411,7 +42430,7 @@
         <v>3272</v>
       </c>
     </row>
-    <row r="332" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>68</v>
       </c>
@@ -42584,7 +42603,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="333" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>68</v>
       </c>
@@ -42640,7 +42659,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="334" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>75</v>
       </c>
@@ -42801,7 +42820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="335" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>75</v>
       </c>
@@ -42980,7 +42999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>75</v>
       </c>
@@ -43156,7 +43175,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="337" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>99</v>
       </c>
@@ -43257,7 +43276,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="338" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>68</v>
       </c>
@@ -43430,7 +43449,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="339" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>68</v>
       </c>
@@ -43492,7 +43511,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="340" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>68</v>
       </c>
@@ -43653,7 +43672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>68</v>
       </c>
@@ -43748,7 +43767,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="342" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>68</v>
       </c>
@@ -43825,7 +43844,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="343" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>99</v>
       </c>
@@ -43998,7 +44017,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="344" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>75</v>
       </c>
@@ -44171,7 +44190,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="345" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>68</v>
       </c>
@@ -44257,7 +44276,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="346" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>99</v>
       </c>
@@ -44361,7 +44380,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="347" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>68</v>
       </c>
@@ -44450,7 +44469,7 @@
         <v>-1708</v>
       </c>
     </row>
-    <row r="348" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>68</v>
       </c>
@@ -44554,7 +44573,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="349" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>99</v>
       </c>
@@ -44649,7 +44668,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="350" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>75</v>
       </c>
@@ -44831,7 +44850,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="351" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>68</v>
       </c>
@@ -44914,7 +44933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="352" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>68</v>
       </c>
@@ -44982,7 +45001,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="353" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>68</v>
       </c>
@@ -45074,7 +45093,7 @@
         <v>-512</v>
       </c>
     </row>
-    <row r="354" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>99</v>
       </c>
@@ -45238,7 +45257,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="355" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>75</v>
       </c>
@@ -45420,7 +45439,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="356" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>68</v>
       </c>
@@ -45527,7 +45546,7 @@
         <v>-1536</v>
       </c>
     </row>
-    <row r="357" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>75</v>
       </c>
@@ -45697,7 +45716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>68</v>
       </c>
@@ -45801,7 +45820,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="359" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>68</v>
       </c>
@@ -45905,7 +45924,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="360" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>99</v>
       </c>
@@ -46084,7 +46103,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="361" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>75</v>
       </c>
@@ -46266,7 +46285,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="362" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>75</v>
       </c>
@@ -46439,7 +46458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="363" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>68</v>
       </c>
@@ -46609,7 +46628,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="364" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>68</v>
       </c>
@@ -46770,7 +46789,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="365" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>99</v>
       </c>
@@ -46931,7 +46950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="366" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>75</v>
       </c>
@@ -47113,7 +47132,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="367" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>99</v>
       </c>
@@ -47295,7 +47314,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="368" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>68</v>
       </c>
@@ -47396,7 +47415,7 @@
         <v>-225</v>
       </c>
     </row>
-    <row r="369" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>68</v>
       </c>
@@ -47500,7 +47519,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="370" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>75</v>
       </c>
@@ -47601,7 +47620,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="371" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>75</v>
       </c>
@@ -47780,7 +47799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="372" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>68</v>
       </c>
@@ -47863,7 +47882,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="373" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>75</v>
       </c>
@@ -47958,7 +47977,7 @@
         <v>-82</v>
       </c>
     </row>
-    <row r="374" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>68</v>
       </c>
@@ -48122,7 +48141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="375" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>75</v>
       </c>
@@ -48199,7 +48218,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="376" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>68</v>
       </c>
@@ -48297,7 +48316,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="377" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>68</v>
       </c>
@@ -48344,7 +48363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="378" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>68</v>
       </c>
@@ -48374,6 +48393,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BR1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>